<commit_message>
New classes added for more readable code
</commit_message>
<xml_diff>
--- a/CourtData.xlsx
+++ b/CourtData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ericsson-my.sharepoint.com/personal/csaba_szabo_ericsson_com/Documents/PycharmProjects/teniszpalya_web_scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_0B099CD80678E4FEE87DD0355E5DCE3AD7CAC4F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E3A41BF-A43F-4A17-802C-1A04BA8AA4DD}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_7AD514674748D6FFE87DD0355E5DCE3AD7CAE4F4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACD830EF-AC8F-43B5-B9FF-7556534DCC64}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Courts" sheetId="1" r:id="rId1"/>
@@ -15809,7 +15809,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15821,6 +15821,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -15840,14 +15848,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -16150,13 +16161,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z770"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O67" workbookViewId="0">
+      <selection activeCell="P87" sqref="P87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
@@ -20252,7 +20263,7 @@
       <c r="N87" t="s">
         <v>629</v>
       </c>
-      <c r="P87" t="s">
+      <c r="P87" s="2" t="s">
         <v>630</v>
       </c>
     </row>
@@ -52283,6 +52294,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P87" r:id="rId1" location="dj-classifieds" xr:uid="{0C43D5C3-4387-4E95-A9DD-53A81427D6D5}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>